<commit_message>
Restructure directories, add initializer for workbooks and worksheets
</commit_message>
<xml_diff>
--- a/exe/Banks.xlsx
+++ b/exe/Banks.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="2" r:id="rId1"/>
-    <sheet name="Wealth" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Accounts" sheetId="2" r:id="rId2"/>
+    <sheet name="Wealth Allocation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Bank Name</t>
   </si>
@@ -31,44 +27,17 @@
     <t>Asset Type</t>
   </si>
   <si>
-    <t>Stock Market</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Bank 1</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>Bank 2</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
     <t>Balance</t>
   </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Emergency</t>
-  </si>
-  <si>
-    <t>Rest</t>
-  </si>
-  <si>
-    <t>Core Saving</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,15 +70,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -375,14 +339,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.66406" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,87 +366,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>150</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787402" bottom="0.787402" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>797.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>217.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare Excel sheets, changed classes and initializing functions
</commit_message>
<xml_diff>
--- a/exe/Banks.xlsx
+++ b/exe/Banks.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B829C8-7828-4565-AF6A-BCB1C75C3ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Accounts" sheetId="2" r:id="rId2"/>
-    <sheet name="Wealth Allocation" sheetId="3" r:id="rId3"/>
+    <sheet name="Accounts" sheetId="2" r:id="rId1"/>
+    <sheet name="Wealth Allocation" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Bank Name</t>
   </si>
@@ -31,13 +48,46 @@
   </si>
   <si>
     <t>Balance</t>
+  </si>
+  <si>
+    <t>Asset Total</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Sparkasse</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>N26</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Rest Collector</t>
+  </si>
+  <si>
+    <t>Core Liquid</t>
+  </si>
+  <si>
+    <t>Emergency Layer</t>
+  </si>
+  <si>
+    <t>Fixed Asset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -70,10 +120,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -339,50 +397,145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>11409.3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>7632.86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>328.61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>4000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>8030.47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>3000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>11409.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1030.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>11409.3</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>